<commit_message>
grid is active with multiple nodes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\DataDrivenGrid\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sami/IdeaProjects/DataDrivenGrid/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -426,9 +429,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -444,7 +447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -465,14 +468,14 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -489,7 +492,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -506,7 +509,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -523,7 +526,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -540,12 +543,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -559,7 +562,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -573,7 +576,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -587,7 +590,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>

</xml_diff>